<commit_message>
se arreglo toda la prgramacion, falta noti y excel
</commit_message>
<xml_diff>
--- a/uploads/usuarios.xlsx
+++ b/uploads/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AVA\serverbienestar\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA99470-DAA5-4AD6-BEF5-ADBDDCD811A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2949A9E-D05A-4EAF-BEE9-061B923DDF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1F56A57F-10CB-4848-9D59-53F2702EC210}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>documento</t>
   </si>
   <si>
-    <t>juan.perez@sena.edu.co</t>
-  </si>
-  <si>
     <t>aria.garcia@sena.edu.co</t>
   </si>
   <si>
@@ -117,16 +114,27 @@
   </si>
   <si>
     <t>Femenino</t>
+  </si>
+  <si>
+    <t>juant.perez@sena.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,8 +178,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -187,11 +196,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,7 +537,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,88 +574,91 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
+      <c r="A2" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="3">
         <v>12345678</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>25</v>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="4">
         <v>87654321</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>26</v>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="3">
         <v>11223344</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>25</v>
+      <c r="H4" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BE10FDE7-79A5-4CA1-861A-2D2EEA8AEF2C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -876,20 +889,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e5c1a488-5979-478c-9cad-90b6f463d0a0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e5c1a488-5979-478c-9cad-90b6f463d0a0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -912,6 +925,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5A85EB4-EBAA-4FAE-8D17-6BC9FA46ABF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1761EA52-29A1-4EE4-9FE3-EEA03631EAB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -926,12 +947,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5A85EB4-EBAA-4FAE-8D17-6BC9FA46ABF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>